<commit_message>
For Testing On linux
Fingers crossed will solve issue #11
</commit_message>
<xml_diff>
--- a/src/dataLoggingTool/dataLogging.xlsx
+++ b/src/dataLoggingTool/dataLogging.xlsx
@@ -27,9 +27,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>Mon Jan 18 23:42:04 2016</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>SP</t>
+  </si>
+  <si>
+    <t>Tue Jan 19 21:58:55 2016</t>
   </si>
 </sst>
 </file>
@@ -95,39 +95,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,142 +206,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -367,7 +391,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -375,103 +399,205 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" width="9.10" max="1"/>
     <col min="2" width="9.10" max="2"/>
     <col min="3" width="9.10" max="3"/>
     <col min="4" width="9.10" max="4"/>
     <col min="5" width="9.10" max="5"/>
+    <col min="6" width="9.10" max="6"/>
   </cols>
   <sheetData>
-    <row spans="1:5" r="1">
-      <c t="s" r="A1">
+    <row spans="1:6" r="2">
+      <c t="s" r="B2">
         <v>1</v>
       </c>
-      <c t="s" r="B1">
+      <c t="s" r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row spans="1:6" r="4">
+      <c t="s" r="B4">
+        <v>2</v>
+      </c>
+      <c t="s" r="C4">
+        <v>4</v>
+      </c>
+      <c t="s" r="D4">
+        <v>0</v>
+      </c>
+      <c t="s" r="E4">
+        <v>5</v>
+      </c>
+      <c t="s" r="F4">
         <v>3</v>
       </c>
     </row>
-    <row spans="1:5" r="3">
-      <c t="s" r="A3">
-        <v>2</v>
-      </c>
-      <c t="s" r="B3">
-        <v>5</v>
-      </c>
-      <c t="s" r="C3">
-        <v>0</v>
-      </c>
-      <c t="s" r="D3">
-        <v>6</v>
-      </c>
-      <c t="s" r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row spans="1:5" r="4">
-      <c t="n" r="A4">
-        <v>0.2519998550415039</v>
-      </c>
-      <c t="n" r="B4">
-        <v>0.00016229636102914804</v>
-      </c>
-      <c t="n" r="C4">
-        <v>0</v>
-      </c>
-      <c t="n" r="D4">
-        <v>40.0</v>
-      </c>
-      <c t="n" r="E4">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row spans="1:5" r="5">
-      <c t="n" r="A5">
-        <v>5.253000020980835</v>
-      </c>
+    <row spans="1:6" r="5">
       <c t="n" r="B5">
-        <v>0.80419928036551191</v>
+        <v>0.009999990463256836</v>
       </c>
       <c t="n" r="C5">
-        <v>0</v>
+        <v>0.001623079702109098</v>
       </c>
       <c t="n" r="D5">
-        <v>40.0</v>
+        <v>0</v>
       </c>
       <c t="n" r="E5">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row spans="1:5" r="6">
-      <c t="n" r="A6">
-        <v>10.251999855041504</v>
-      </c>
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F5">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="6">
       <c t="n" r="B6">
-        <v>1.4529936558417083</v>
+        <v>5.008999824523926</v>
       </c>
       <c t="n" r="C6">
-        <v>0</v>
+        <v>0.8057030783116591</v>
       </c>
       <c t="n" r="D6">
-        <v>40.0</v>
+        <v>0</v>
       </c>
       <c t="n" r="E6">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row spans="1:5" r="7">
-      <c t="n" r="A7">
-        <v>15.250999927520752</v>
-      </c>
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F6">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="7">
       <c t="n" r="B7">
-        <v>2.0459098480726179</v>
+        <v>10.013999938964844</v>
       </c>
       <c t="n" r="C7">
-        <v>0</v>
+        <v>1.4552532560529658</v>
       </c>
       <c t="n" r="D7">
-        <v>40.0</v>
+        <v>0</v>
       </c>
       <c t="n" r="E7">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F7">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="8">
+      <c t="n" r="B8">
+        <v>15.020999908447266</v>
+      </c>
+      <c t="n" r="C8">
+        <v>2.0490455230282096</v>
+      </c>
+      <c t="n" r="D8">
+        <v>0</v>
+      </c>
+      <c t="n" r="E8">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F8">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="9">
+      <c t="n" r="B9">
+        <v>20.024999856948853</v>
+      </c>
+      <c t="n" r="C9">
+        <v>2.6015915356791788</v>
+      </c>
+      <c t="n" r="D9">
+        <v>0</v>
+      </c>
+      <c t="n" r="E9">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F9">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="10">
+      <c t="n" r="B10">
+        <v>25.032999992370605</v>
+      </c>
+      <c t="n" r="C10">
+        <v>3.1216525842401648</v>
+      </c>
+      <c t="n" r="D10">
+        <v>0</v>
+      </c>
+      <c t="n" r="E10">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F10">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="11">
+      <c t="n" r="B11">
+        <v>30.039999961853027</v>
+      </c>
+      <c t="n" r="C11">
+        <v>3.6136476695203998</v>
+      </c>
+      <c t="n" r="D11">
+        <v>0</v>
+      </c>
+      <c t="n" r="E11">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F11">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="12">
+      <c t="n" r="B12">
+        <v>35.04099988937378</v>
+      </c>
+      <c t="n" r="C12">
+        <v>4.0807550146510385</v>
+      </c>
+      <c t="n" r="D12">
+        <v>0</v>
+      </c>
+      <c t="n" r="E12">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F12">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="13">
+      <c t="n" r="B13">
+        <v>40.04099988937378</v>
+      </c>
+      <c t="n" r="C13">
+        <v>4.5262327279041648</v>
+      </c>
+      <c t="n" r="D13">
+        <v>0</v>
+      </c>
+      <c t="n" r="E13">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F13">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row spans="1:6" r="14">
+      <c t="n" r="B14">
+        <v>45.04099988937378</v>
+      </c>
+      <c t="n" r="C14">
+        <v>4.9522529304685978</v>
+      </c>
+      <c t="n" r="D14">
+        <v>0</v>
+      </c>
+      <c t="n" r="E14">
+        <v>40.0</v>
+      </c>
+      <c t="n" r="F14">
         <v>0.35</v>
       </c>
     </row>

</xml_diff>